<commit_message>
Excel Read And Write function
</commit_message>
<xml_diff>
--- a/download.xlsx
+++ b/download.xlsx
@@ -1,47 +1,71 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="2" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>Sl</t>
+  </si>
+  <si>
+    <t>e1</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Sallary</t>
+  </si>
+  <si>
+    <t>WD</t>
+  </si>
+  <si>
+    <t>Aman</t>
+  </si>
+  <si>
+    <t>6790</t>
+  </si>
+  <si>
+    <t>Krishna</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Jyoti</t>
+  </si>
+  <si>
+    <t>Suresh</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>Kashyap</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -65,13 +89,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -395,135 +427,154 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>sno</v>
-      </c>
-      <c r="B1" t="str">
-        <v>fruit_name</v>
-      </c>
-      <c r="C1" t="str">
-        <v>color</v>
-      </c>
-      <c r="D1" t="str">
-        <v>price</v>
-      </c>
-      <c r="E1" t="str">
-        <v>season</v>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="str">
-        <v>Mango</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Yellow</v>
-      </c>
-      <c r="D2">
-        <v>299</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Summer</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>1001</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="str">
-        <v>Apple</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Red</v>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>1002</v>
       </c>
       <c r="D3">
-        <v>345</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Winter</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>4000</v>
+      </c>
+      <c r="E3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="str">
-        <v>Papaya</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Orange</v>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>1003</v>
       </c>
       <c r="D4">
-        <v>187</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Spring</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>3000</v>
+      </c>
+      <c r="E4">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="str">
-        <v>Banana</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Yellow</v>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>1004</v>
       </c>
       <c r="D5">
-        <v>69</v>
-      </c>
-      <c r="E5" t="str">
-        <v>All</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>2000</v>
+      </c>
+      <c r="E5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="str">
-        <v>Kivi</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Green</v>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>1005</v>
       </c>
       <c r="D6">
-        <v>399</v>
-      </c>
-      <c r="E6" t="str">
-        <v>Winter</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>1000</v>
+      </c>
+      <c r="E6">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="str">
-        <v>Orange</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Orange</v>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>1006</v>
       </c>
       <c r="D7">
-        <v>199</v>
-      </c>
-      <c r="E7" t="str">
-        <v>Summer</v>
+        <v>5000</v>
+      </c>
+      <c r="E7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>1007</v>
+      </c>
+      <c r="D8">
+        <v>4000</v>
+      </c>
+      <c r="E8">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E7"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>